<commit_message>
update markerset to logtrack properties
</commit_message>
<xml_diff>
--- a/wi-properties.xlsx
+++ b/wi-properties.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="106">
   <si>
     <t>class</t>
   </si>
@@ -180,9 +180,6 @@
     <t>wifamily</t>
   </si>
   <si>
-    <t>logtrack</t>
-  </si>
-  <si>
     <t>showTitle</t>
   </si>
   <si>
@@ -279,9 +276,6 @@
     <t>ZoneSet</t>
   </si>
   <si>
-    <t>Zonation</t>
-  </si>
-  <si>
     <t>wizoneset</t>
   </si>
   <si>
@@ -292,6 +286,54 @@
   </si>
   <si>
     <t>Width (inchs)</t>
+  </si>
+  <si>
+    <t>zoneset</t>
+  </si>
+  <si>
+    <t>zone</t>
+  </si>
+  <si>
+    <t>showName</t>
+  </si>
+  <si>
+    <t>showOnTrack</t>
+  </si>
+  <si>
+    <t>Show Name</t>
+  </si>
+  <si>
+    <t>Show On Track</t>
+  </si>
+  <si>
+    <t>Options</t>
+  </si>
+  <si>
+    <t>d3-logtrack</t>
+  </si>
+  <si>
+    <t>wiref</t>
+  </si>
+  <si>
+    <t>refSpec</t>
+  </si>
+  <si>
+    <t>well.bottomDepth</t>
+  </si>
+  <si>
+    <t>well.topDepth</t>
+  </si>
+  <si>
+    <t>markerSet</t>
+  </si>
+  <si>
+    <t>MarkerSet</t>
+  </si>
+  <si>
+    <t>Zonation &amp; MarkerSet</t>
+  </si>
+  <si>
+    <t>wimarkerset</t>
   </si>
 </sst>
 </file>
@@ -637,21 +679,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -670,8 +714,11 @@
       <c r="F1" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -688,7 +735,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -705,7 +752,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -722,7 +769,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -739,7 +786,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -756,7 +803,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -773,7 +820,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -790,7 +837,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>52</v>
       </c>
@@ -806,8 +853,17 @@
       <c r="E9" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>98</v>
+      </c>
+      <c r="G9" t="s">
+        <v>100</v>
+      </c>
+      <c r="H9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>52</v>
       </c>
@@ -823,8 +879,17 @@
       <c r="E10" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>98</v>
+      </c>
+      <c r="G10" t="s">
+        <v>101</v>
+      </c>
+      <c r="H10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>52</v>
       </c>
@@ -841,7 +906,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>52</v>
       </c>
@@ -858,7 +923,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>52</v>
       </c>
@@ -875,7 +940,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -892,7 +957,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>52</v>
       </c>
@@ -909,7 +974,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>52</v>
       </c>
@@ -943,7 +1008,7 @@
         <v>19</v>
       </c>
       <c r="F17" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1070,257 +1135,385 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>97</v>
+      </c>
+      <c r="B25" t="s">
         <v>54</v>
       </c>
-      <c r="B25" t="s">
-        <v>55</v>
-      </c>
       <c r="C25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D25" t="s">
         <v>15</v>
       </c>
       <c r="E25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>54</v>
+        <v>97</v>
       </c>
       <c r="B26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D26" t="s">
         <v>15</v>
       </c>
       <c r="E26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>54</v>
+        <v>97</v>
       </c>
       <c r="B27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D27" t="s">
         <v>15</v>
       </c>
       <c r="E27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>54</v>
+        <v>97</v>
       </c>
       <c r="B28" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D28" t="s">
         <v>15</v>
       </c>
       <c r="E28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>54</v>
+        <v>97</v>
       </c>
       <c r="B29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C29" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D29" t="s">
         <v>15</v>
       </c>
       <c r="E29" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F29" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>54</v>
+        <v>97</v>
       </c>
       <c r="B30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D30" t="s">
         <v>15</v>
       </c>
       <c r="E30" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F30" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>54</v>
+        <v>97</v>
       </c>
       <c r="B31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C31" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D31" t="s">
         <v>15</v>
       </c>
       <c r="E31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>54</v>
+        <v>97</v>
       </c>
       <c r="B32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C32" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D32" t="s">
         <v>15</v>
       </c>
       <c r="E32" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>97</v>
       </c>
       <c r="B33" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C33" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D33" t="s">
         <v>15</v>
       </c>
       <c r="E33" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>54</v>
+        <v>97</v>
       </c>
       <c r="B34" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D34" t="s">
         <v>15</v>
       </c>
       <c r="E34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F34" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>54</v>
+        <v>97</v>
       </c>
       <c r="B35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D35" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>54</v>
+        <v>97</v>
       </c>
       <c r="B36" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D36" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>54</v>
+        <v>97</v>
       </c>
       <c r="B37" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C37" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D37" t="s">
         <v>15</v>
       </c>
       <c r="E37" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>54</v>
+        <v>97</v>
       </c>
       <c r="B38" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="C38" t="s">
-        <v>86</v>
+        <v>103</v>
       </c>
       <c r="D38" t="s">
         <v>15</v>
       </c>
       <c r="E38" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="F38" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>54</v>
+        <v>97</v>
       </c>
       <c r="B39" t="s">
+        <v>88</v>
+      </c>
+      <c r="C39" t="s">
+        <v>85</v>
+      </c>
+      <c r="D39" t="s">
+        <v>15</v>
+      </c>
+      <c r="E39" t="s">
+        <v>104</v>
+      </c>
+      <c r="F39" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>97</v>
+      </c>
+      <c r="B40" t="s">
+        <v>67</v>
+      </c>
+      <c r="D40" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>90</v>
+      </c>
+      <c r="B41" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" t="s">
+        <v>12</v>
+      </c>
+      <c r="D41" t="s">
+        <v>15</v>
+      </c>
+      <c r="E41" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>91</v>
+      </c>
+      <c r="B42" t="s">
+        <v>6</v>
+      </c>
+      <c r="C42" t="s">
+        <v>12</v>
+      </c>
+      <c r="D42" t="s">
+        <v>15</v>
+      </c>
+      <c r="E42" t="s">
         <v>68</v>
       </c>
-      <c r="D39" t="s">
-        <v>74</v>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>91</v>
+      </c>
+      <c r="B43" t="s">
+        <v>25</v>
+      </c>
+      <c r="C43" t="s">
+        <v>37</v>
+      </c>
+      <c r="D43" t="s">
+        <v>16</v>
+      </c>
+      <c r="E43" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>91</v>
+      </c>
+      <c r="B44" t="s">
+        <v>26</v>
+      </c>
+      <c r="C44" t="s">
+        <v>38</v>
+      </c>
+      <c r="D44" t="s">
+        <v>16</v>
+      </c>
+      <c r="E44" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>91</v>
+      </c>
+      <c r="B45" t="s">
+        <v>92</v>
+      </c>
+      <c r="C45" t="s">
+        <v>94</v>
+      </c>
+      <c r="D45" t="s">
+        <v>15</v>
+      </c>
+      <c r="E45" t="s">
+        <v>96</v>
+      </c>
+      <c r="F45" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>91</v>
+      </c>
+      <c r="B46" t="s">
+        <v>93</v>
+      </c>
+      <c r="C46" t="s">
+        <v>95</v>
+      </c>
+      <c r="D46" t="s">
+        <v>15</v>
+      </c>
+      <c r="E46" t="s">
+        <v>96</v>
+      </c>
+      <c r="F46" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>